<commit_message>
ExcelParser + ImportQueryGenerator + Excel files: no more ID needed
Updated Burgen xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/BurgenVisitSmall.xlsx
+++ b/src/test/resources/BurgenVisitSmall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEDF125-C864-A040-90BE-84278C00BB39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D7F5F3-FF5C-4E9E-9EE2-5B7006CAE0B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Architecture" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Schlagwort</t>
-  </si>
-  <si>
-    <t>Objekt 1</t>
   </si>
   <si>
     <t xml:space="preserve">Herzogskasten Abensberg </t>
@@ -106,9 +103,6 @@
   </si>
   <si>
     <t>https://www.alleburgen.de/bd.php?id=5136</t>
-  </si>
-  <si>
-    <t>Objekt 2</t>
   </si>
   <si>
     <t>Schloss Aicha vorm Wald</t>
@@ -136,9 +130,6 @@
   </si>
   <si>
     <t>Deutschland, Bayern, Niederbayern, Landkreis Passau</t>
-  </si>
-  <si>
-    <t>Objekt 10</t>
   </si>
   <si>
     <t>Alte Residenz Passau</t>
@@ -824,11 +815,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -890,8 +878,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -940,7 +928,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1260,958 +1248,944 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B62047-7F58-5A46-866E-64350EDAC560}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>186</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1450</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="128" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" ht="350" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="350" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B15" s="9">
-        <v>1450</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1500</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" s="9">
-        <v>1500</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>190</v>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>193</v>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>193</v>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>193</v>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-    </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>193</v>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
     </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-    </row>
-    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-    </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="19" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-    </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-    </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-    </row>
-    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>193</v>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
     </row>
-    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-    </row>
-    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-    </row>
-    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-    </row>
-    <row r="74" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="19" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-    </row>
-    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-    </row>
-    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-    </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>193</v>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
     </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-    </row>
-    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-    </row>
-    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-    </row>
-    <row r="84" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="19" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-    </row>
-    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-    </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-    </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-    </row>
-    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>193</v>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+    </row>
+    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
     </row>
-    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-    </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-    </row>
-    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-    </row>
-    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-    </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="16" t="s">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
-    </row>
-    <row r="95" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+    </row>
+    <row r="94" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B94" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D94" s="8"/>
+    </row>
+    <row r="95" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96" s="16"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B98" s="8">
+        <v>55</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+    </row>
+    <row r="101" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B102" s="6"/>
+      <c r="C102" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D95" s="9"/>
-    </row>
-    <row r="96" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="19" t="s">
+      <c r="D102" s="10"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B97" s="17"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-    </row>
-    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-    </row>
-    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B99" s="9">
-        <v>55</v>
-      </c>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-    </row>
-    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-    </row>
-    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-    </row>
-    <row r="102" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D102" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B103" s="7"/>
-      <c r="C103" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D103" s="11"/>
-    </row>
-    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B104" s="7"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-    </row>
-    <row r="105" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-    </row>
-    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-    </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-    </row>
-    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B108" s="7"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-    </row>
-    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B109" s="7"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104" s="6"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B106" s="6"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B108" s="6"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B102" r:id="rId1" xr:uid="{0C360D41-CA25-2443-A2CC-09A19BFCDDCA}"/>
-    <hyperlink ref="C102" r:id="rId2" xr:uid="{113EE543-CF0E-EB42-B16C-9A7CD17C4A6C}"/>
-    <hyperlink ref="C103" r:id="rId3" xr:uid="{A7B5D0A1-4405-BF4C-AD51-FDB6DA67A17C}"/>
-    <hyperlink ref="D102" r:id="rId4" xr:uid="{A473B796-85F0-3C42-8CB6-8217AB7A1B41}"/>
+    <hyperlink ref="B101" r:id="rId1" xr:uid="{0C360D41-CA25-2443-A2CC-09A19BFCDDCA}"/>
+    <hyperlink ref="C101" r:id="rId2" xr:uid="{113EE543-CF0E-EB42-B16C-9A7CD17C4A6C}"/>
+    <hyperlink ref="C102" r:id="rId3" xr:uid="{A7B5D0A1-4405-BF4C-AD51-FDB6DA67A17C}"/>
+    <hyperlink ref="D101" r:id="rId4" xr:uid="{A473B796-85F0-3C42-8CB6-8217AB7A1B41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2225,99 +2199,99 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+    <row r="8" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2327,31 +2301,31 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{3AE5E07F-03A4-C44A-95BF-B8A2F409ADF3}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Reference'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Reference'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B16:SG16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{C168F23A-318E-8E4F-AD73-11854368A096}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Object'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Object'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B12:SG12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{148BF1E5-800F-BE4C-9549-CEBC6F8ADC94}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B11:SG11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{94A1A3BC-6843-004A-A52D-F69435435B65}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Person'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Person'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B10:SG10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{F3FAC391-660F-6C4A-9716-00E9FDAFB56F}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Place'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Place'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B9:SG9</xm:sqref>
         </x14:dataValidation>
@@ -2369,89 +2343,89 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>63</v>
+    <row r="14" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2461,19 +2435,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{7FF46B0C-F374-CF42-A2EB-0029AE3E89CC}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Reference'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Reference'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B15:SG15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{A8094F4E-BB51-0940-84F5-7C89A42326AD}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B4:SG7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{C3A775AA-77C8-3342-B68A-81CDFE216824}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Object'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Object'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B3:SG3 B11:SG12</xm:sqref>
         </x14:dataValidation>
@@ -2491,142 +2465,142 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:1" s="19" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+    <row r="7" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+    <row r="9" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="16" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+    <row r="18" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+    <row r="19" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+    <row r="20" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+    <row r="22" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+    <row r="23" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+    <row r="24" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+    <row r="25" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+    <row r="26" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2638,43 +2612,43 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{693FABEF-AC10-C64B-9B21-1A82D9E3C93D}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Activity'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Activity'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B24:SG24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{2ED00E7D-F593-1845-BE13-A56C1E04E412}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Group'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Group'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B22:SG22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{88ADABAD-8122-5D43-A0D5-165BD16178CF}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B21:SG21</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{56306C6B-0078-5A48-AC9D-F6D03FD45049}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Object'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Object'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B20:SG20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{A34F9EB7-401D-CB42-8047-ABF7380F7D06}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Institution'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Institution'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B13:SG14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{B13B3CAA-587B-A844-9414-9F1B842A96EF}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Place'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Place'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B8:SG8 B25:SG25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{6683BB6A-C4FB-7A49-AC4C-7ADF6BBDFA5D}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Person'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Person'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B7:SG7 B23:SG23</xm:sqref>
         </x14:dataValidation>
@@ -2692,304 +2666,304 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+    <row r="8" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+    <row r="9" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+    <row r="18" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+    <row r="19" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+    <row r="20" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+    <row r="21" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+    <row r="22" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+    <row r="23" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+    <row r="24" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+    <row r="25" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+    <row r="26" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+    <row r="27" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+    <row r="28" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+    <row r="29" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+    <row r="30" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+    <row r="31" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+    <row r="32" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="37" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="38" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="39" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24" t="s">
+    <row r="40" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="25" t="s">
+    <row r="41" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
+    <row r="42" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="s">
+    <row r="43" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
+    <row r="44" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="27" t="s">
+    <row r="45" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="28" t="s">
+    <row r="46" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="21" t="s">
+    <row r="47" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24" t="s">
+    <row r="56" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3004,43 +2978,43 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{3C5F7A7F-6C8F-894F-86F3-51D8515C1CEE}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Reference'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Reference'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B57:SG57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{6B283EB1-2B55-0246-A425-29F256BB0FC3}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Activity'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Activity'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B49:SG49 B53:SG53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{923CDD18-E90B-E348-B9B9-EE5E29DF4FEF}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B36:SG36 B51:SG51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{48A7218D-97EA-8944-BDC6-CBDAA50F6F9D}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Institution'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Institution'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B33:SG33 B35:SG35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{F532946B-8E9D-E341-AA33-3C3E57489699}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Place'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Place'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B21:SG21 B52:SG52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{44CC7895-0AEE-174E-BC1C-897BBBE8E0AA}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Group'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Group'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B15:SG15 B47:SG47 B45:SG45</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{A8E2B8B5-1AB9-0C4D-9D79-7C5307BF52BD}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Person'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Person'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B14:SG14 B50:SG50 B46:SG46 B44:SG44</xm:sqref>
         </x14:dataValidation>
@@ -3058,49 +3032,49 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3110,19 +3084,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{C1E54705-5221-1148-A5E1-14237BC13ECB}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Reference'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Reference'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B6:SG7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{9C82D88E-5D57-4042-9FDF-2F91344A5CF4}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Place'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Place'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B4:SG4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{9A23AA8B-7508-284F-B5C4-D6CE919B09C4}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B3:SG3</xm:sqref>
         </x14:dataValidation>
@@ -3140,284 +3114,284 @@
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+    <row r="10" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+    <row r="14" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+    <row r="15" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="21" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+    <row r="16" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+    <row r="17" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+    <row r="18" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="21" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+    <row r="30" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+    <row r="31" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+    <row r="32" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+    <row r="33" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+    <row r="34" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="26" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="28" t="s">
+    <row r="35" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="26" t="s">
+    <row r="36" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="s">
+    <row r="37" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="28" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+    <row r="51" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3432,31 +3406,31 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{FB93C19A-10BB-294E-BCE2-D56B8E3B9481}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Reference'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Reference'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B52:SG52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{A4D2FDE9-F4B2-A44C-9A75-A30FEF355AF6}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Object'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Object'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B55:SG55 B47:SG48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{6F3A47BD-445C-214C-956D-0B1DBEE109CB}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Activity'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Activity'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B40:SG40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{8B425E0E-2D8E-E542-9EFE-7A8573553CF9}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B39:SG39 B41:SG43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{748C32FB-9A0A-7547-A609-027C5E30BA8C}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Place'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Place'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B13:SG13 B22:SG22</xm:sqref>
         </x14:dataValidation>
@@ -3474,79 +3448,79 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3556,31 +3530,31 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{3F0A9DD4-0A05-E24A-A56B-E2EF1A777777}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Object'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Object'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B14:SG14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{5D59929F-CD85-344C-9523-C89EE1BCE887}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Reference'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Reference'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B11:SG11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{7E43ED23-C0C2-BC45-BE98-93EB12E4E309}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Person'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Person'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B6:SG7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{F4729C01-0C11-F646-9DFB-C9112EA95B4F}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Activity'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Activity'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B5:SG5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{31CB38D9-4C9D-E440-BD40-45FF819239BE}">
           <x14:formula1>
-            <xm:f>'/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/[visitExcel.xlsx]Architecture'!#REF!</xm:f>
+            <xm:f>'C:\Users\Manu\IdeaProjects\MetaDBRestAPIPadim\templates\[visitExcel.xlsx]Architecture'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B4:SG4</xm:sqref>
         </x14:dataValidation>

</xml_diff>